<commit_message>
Further explanations in the .py Code
Explaining the linear regression and ARIMA regression
</commit_message>
<xml_diff>
--- a/monhtly_forex_rates.xlsx
+++ b/monhtly_forex_rates.xlsx
@@ -155,11 +155,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1157080671"/>
-        <c:axId val="389385508"/>
+        <c:axId val="1003804404"/>
+        <c:axId val="694588706"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1157080671"/>
+        <c:axId val="1003804404"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -211,10 +211,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="389385508"/>
+        <c:crossAx val="694588706"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="389385508"/>
+        <c:axId val="694588706"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="14000.0"/>
@@ -290,7 +290,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1157080671"/>
+        <c:crossAx val="1003804404"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>